<commit_message>
edits to demand figure for chapter 7
</commit_message>
<xml_diff>
--- a/indmarketdemand/preventative_healthcare.xlsx
+++ b/indmarketdemand/preventative_healthcare.xlsx
@@ -1,73 +1,80 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrietbrookesgray/Documents/GitHub/bfh-textbook/indmarketdemand/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C54317D-6955-8948-887D-FF3B9B4A5D75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26380" windowHeight="15920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t xml:space="preserve">x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$0.4 clorin (Kenya 2004)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$2 deworming (Kenya 2001)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$7 bednets (Kenya 2007, pregnant women)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$2 soap (Uganda 2009)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$15 water filters (Ghana 2009)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$1 vitamin (India 2009)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$7 bednets (Kenya 2007)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$5 cement latrine slabs (Tanzania 2015)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$2 vitamins (Uganda 2009)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$15 plastic latrine slab (Tanzania 2015)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$2 soap (Guatemala 2009) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">$0.26 clorin (Zambia 2006)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$2 vitamins (Guatemala 2009)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>Clorin (Kenya 2004)</t>
+  </si>
+  <si>
+    <t>Deworming (Kenya 2001)</t>
+  </si>
+  <si>
+    <t>Bednets (Kenya 2007, pregnant women)</t>
+  </si>
+  <si>
+    <t>Soap (Uganda 2009)</t>
+  </si>
+  <si>
+    <t>Water filters (Ghana 2009)</t>
+  </si>
+  <si>
+    <t>Vitamin (India 2009)</t>
+  </si>
+  <si>
+    <t>Bednets (Kenya 2007)</t>
+  </si>
+  <si>
+    <t>Cement latrine slabs (Tanzania 2015)</t>
+  </si>
+  <si>
+    <t>Vitamins (Uganda 2009)</t>
+  </si>
+  <si>
+    <t>Plastic latrine slab (Tanzania 2015)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soap (Guatemala 2009) </t>
+  </si>
+  <si>
+    <t>Clorin (Zambia 2006)</t>
+  </si>
+  <si>
+    <t>Vitamins (Guatemala 2009)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -103,6 +110,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -384,14 +400,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44:C46"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,496 +420,496 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>0.00800744878957216</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.600569306930693</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>8.0074487895721597E-3</v>
+      </c>
+      <c r="B2">
+        <v>0.60056930693069299</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>0.195716945996276</v>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.19571694599627601</v>
+      </c>
+      <c r="B3">
         <v>0.103118811881188</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>0.300000000000001</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.0198019801980198</v>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0.30000000000000099</v>
+      </c>
+      <c r="B4">
+        <v>1.9801980198019799E-2</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>0.00800744878957216</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.7525</v>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>8.0074487895721597E-3</v>
+      </c>
+      <c r="B5">
+        <v>0.75249999999999995</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>0.404283054003725</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>0.171732673267327</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>0.00800744878957216</v>
-      </c>
-      <c r="B7" t="n">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>8.0074487895721597E-3</v>
+      </c>
+      <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>0.206145251396649</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.914232673267326</v>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0.20614525139664899</v>
+      </c>
+      <c r="B8">
+        <v>0.91423267326732605</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>0.300000000000001</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.813762376237624</v>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0.30000000000000099</v>
+      </c>
+      <c r="B9">
+        <v>0.81376237623762404</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>0.602420856610801</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.382475247524752</v>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0.60242085661080103</v>
+      </c>
+      <c r="B10">
+        <v>0.38247524752475198</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>0.498137802607077</v>
-      </c>
-      <c r="B11" t="n">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0.49813780260707702</v>
+      </c>
+      <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>0.998696461824954</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0.958341584158416</v>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0.99869646182495397</v>
+      </c>
+      <c r="B12">
+        <v>0.95834158415841597</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="n">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>1.48882681564246</v>
       </c>
-      <c r="B13" t="n">
-        <v>0.909331683168317</v>
+      <c r="B13">
+        <v>0.90933168316831703</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>1.39497206703911</v>
-      </c>
-      <c r="B14" t="n">
-        <v>0.909331683168317</v>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1.3949720670391099</v>
+      </c>
+      <c r="B14">
+        <v>0.90933168316831703</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>2.89664804469274</v>
-      </c>
-      <c r="B15" t="n">
-        <v>0.48049504950495</v>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2.8966480446927401</v>
+      </c>
+      <c r="B15">
+        <v>0.48049504950494998</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>4.28361266294227</v>
-      </c>
-      <c r="B16" t="n">
-        <v>0.24279702970297</v>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>4.2836126629422697</v>
+      </c>
+      <c r="B16">
+        <v>0.24279702970297001</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>5.77486033519553</v>
-      </c>
-      <c r="B17" t="n">
-        <v>0.0810643564356436</v>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>5.7748603351955303</v>
+      </c>
+      <c r="B17">
+        <v>8.1064356435643595E-2</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>0.300000000000001</v>
-      </c>
-      <c r="B18" t="n">
-        <v>0.72799504950495</v>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>0.30000000000000099</v>
+      </c>
+      <c r="B18">
+        <v>0.72799504950494998</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>0.498137802607077</v>
-      </c>
-      <c r="B19" t="n">
-        <v>0.72799504950495</v>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0.49813780260707702</v>
+      </c>
+      <c r="B19">
+        <v>0.72799504950494998</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>0.998696461824954</v>
-      </c>
-      <c r="B20" t="n">
-        <v>0.561361386138614</v>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0.99869646182495397</v>
+      </c>
+      <c r="B20">
+        <v>0.56136138613861397</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>0.498137802607077</v>
-      </c>
-      <c r="B21" t="n">
-        <v>0.74759900990099</v>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>0.49813780260707702</v>
+      </c>
+      <c r="B21">
+        <v>0.74759900990099004</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>0.696275605214153</v>
-      </c>
-      <c r="B22" t="n">
-        <v>0.627524752475247</v>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>0.69627560521415299</v>
+      </c>
+      <c r="B22">
+        <v>0.62752475247524697</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="n">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>1.49925512104283</v>
       </c>
-      <c r="B23" t="n">
-        <v>0.335915841584158</v>
+      <c r="B23">
+        <v>0.33591584158415799</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="n">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>1.89553072625698</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>0.24769801980198</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>2.88621973929237</v>
-      </c>
-      <c r="B25" t="n">
-        <v>0.176633663366337</v>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2.8862197392923701</v>
+      </c>
+      <c r="B25">
+        <v>0.17663366336633701</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>0.498137802607077</v>
-      </c>
-      <c r="B26" t="n">
-        <v>0.659381188118812</v>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>0.49813780260707702</v>
+      </c>
+      <c r="B26">
+        <v>0.65938118811881197</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="n">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
         <v>1.19683426443203</v>
       </c>
-      <c r="B27" t="n">
-        <v>0.441287128712871</v>
+      <c r="B27">
+        <v>0.44128712871287101</v>
       </c>
       <c r="C27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>1.98938547486034</v>
-      </c>
-      <c r="B28" t="n">
-        <v>0.311410891089109</v>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1.9893854748603399</v>
+      </c>
+      <c r="B28">
+        <v>0.31141089108910902</v>
       </c>
       <c r="C28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>2.68808193668529</v>
-      </c>
-      <c r="B29" t="n">
-        <v>0.301608910891089</v>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2.6880819366852902</v>
+      </c>
+      <c r="B29">
+        <v>0.30160891089108899</v>
       </c>
       <c r="C29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="n">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
         <v>3.38677839851024</v>
       </c>
-      <c r="B30" t="n">
-        <v>0.250148514851485</v>
+      <c r="B30">
+        <v>0.25014851485148498</v>
       </c>
       <c r="C30" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="n">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
         <v>4.0854748603352</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31">
         <v>0.181534653465347</v>
       </c>
       <c r="C31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>0.498137802607077</v>
-      </c>
-      <c r="B32" t="n">
-        <v>0.931386138613861</v>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>0.49813780260707702</v>
+      </c>
+      <c r="B32">
+        <v>0.93138613861386099</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>0.998696461824954</v>
-      </c>
-      <c r="B33" t="n">
-        <v>0.828465346534653</v>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>0.99869646182495397</v>
+      </c>
+      <c r="B33">
+        <v>0.82846534653465298</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="n">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>1.48882681564246</v>
       </c>
-      <c r="B34" t="n">
-        <v>0.580965346534653</v>
+      <c r="B34">
+        <v>0.58096534653465304</v>
       </c>
       <c r="C34" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="n">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
         <v>1.48882681564246</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35">
         <v>0.571163366336634</v>
       </c>
       <c r="C35" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>3.67877094972067</v>
-      </c>
-      <c r="B36" t="n">
-        <v>0.318762376237624</v>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>3.6787709497206702</v>
+      </c>
+      <c r="B36">
+        <v>0.31876237623762399</v>
       </c>
       <c r="C36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>5.87914338919926</v>
-      </c>
-      <c r="B37" t="n">
-        <v>0.208490099009901</v>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>5.8791433891992604</v>
+      </c>
+      <c r="B37">
+        <v>0.20849009900990101</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>0.498137802607077</v>
-      </c>
-      <c r="B38" t="n">
-        <v>0.821113861386139</v>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>0.49813780260707702</v>
+      </c>
+      <c r="B38">
+        <v>0.82111386138613895</v>
       </c>
       <c r="C38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>0.998696461824954</v>
-      </c>
-      <c r="B39" t="n">
-        <v>0.72799504950495</v>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>0.99869646182495397</v>
+      </c>
+      <c r="B39">
+        <v>0.72799504950494998</v>
       </c>
       <c r="C39" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="n">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
         <v>1.49925512104283</v>
       </c>
-      <c r="B40" t="n">
-        <v>0.551559405940594</v>
+      <c r="B40">
+        <v>0.55155940594059405</v>
       </c>
       <c r="C40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="n">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
         <v>0.101862197392924</v>
       </c>
-      <c r="B41" t="n">
-        <v>0.781905940594059</v>
+      <c r="B41">
+        <v>0.78190594059405905</v>
       </c>
       <c r="C41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>0.195716945996276</v>
-      </c>
-      <c r="B42" t="n">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>0.19571694599627601</v>
+      </c>
+      <c r="B42">
         <v>0.502549504950495</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>0.300000000000001</v>
-      </c>
-      <c r="B43" t="n">
-        <v>0.529504950495049</v>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>0.30000000000000099</v>
+      </c>
+      <c r="B43">
+        <v>0.52950495049504898</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>0.487709497206704</v>
-      </c>
-      <c r="B44" t="n">
-        <v>0.799059405940594</v>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>0.48770949720670398</v>
+      </c>
+      <c r="B44">
+        <v>0.79905940594059399</v>
       </c>
       <c r="C44" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>0.998696461824954</v>
-      </c>
-      <c r="B45" t="n">
-        <v>0.781905940594059</v>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>0.99869646182495397</v>
+      </c>
+      <c r="B45">
+        <v>0.78190594059405905</v>
       </c>
       <c r="C45" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="n">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
         <v>1.49925512104283</v>
       </c>
-      <c r="B46" t="n">
-        <v>0.590767326732673</v>
+      <c r="B46">
+        <v>0.59076732673267296</v>
       </c>
       <c r="C46" t="s">
         <v>15</v>
@@ -899,6 +917,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>